<commit_message>
carbon market too hard mabn
</commit_message>
<xml_diff>
--- a/markets.xlsx
+++ b/markets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheikh M Ahmed\modelling_MCDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8592D4-C6DF-42EF-90D3-1062082F2C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F809AD03-70D0-46CE-9A71-06E7462A34B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{5524CA32-E132-410D-B865-513BEFDAB590}"/>
   </bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D915BB96-A88E-4797-BAC2-270B960E39C0}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,7 +417,7 @@
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -437,342 +437,333 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(20,40)/100</f>
-        <v>0.32</v>
+        <v>0.4</v>
       </c>
       <c r="C2">
         <f ca="1">B2*0.5</f>
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(5,15)/100</f>
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E2">
         <f ca="1">D2*0.5</f>
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
         <f ca="1">RANDBETWEEN(90,120)</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <f ca="1">RANDBETWEEN(20,40)/100</f>
-        <v>0.27</v>
+        <v>0.34</v>
       </c>
       <c r="C3">
         <f ca="1">B3*0.5</f>
-        <v>0.13500000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D25" ca="1" si="0">RANDBETWEEN(5,15)/100</f>
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E25" ca="1" si="1">D3*0.5</f>
-        <v>2.5000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F25" ca="1" si="2">RANDBETWEEN(90,120)</f>
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B25" ca="1" si="3">RANDBETWEEN(20,40)/100</f>
+        <f t="shared" ref="B4:B25" ca="1" si="2">RANDBETWEEN(20,40)/100</f>
         <v>0.32</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C25" ca="1" si="4">B4*0.5</f>
+        <f t="shared" ref="C4:C25" ca="1" si="3">B4*0.5</f>
         <v>0.16</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F4">
-        <f t="shared" ca="1" si="2"/>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.4</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.34</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.17</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.08</v>
+        <v>0.13</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.04</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="2"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.38</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.19</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4999999999999997E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.25</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.4</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.125</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.2</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4999999999999997E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="2"/>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.32</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.15</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.16</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.04</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="2"/>
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.23</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.115</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F9">
-        <f t="shared" ca="1" si="2"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.28000000000000003</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.23</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.14000000000000001</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.115</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.05</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F10">
-        <f t="shared" ca="1" si="2"/>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.27</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.2</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.13500000000000001</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.1</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4999999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F11">
-        <f t="shared" ca="1" si="2"/>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.39</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.19500000000000001</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4999999999999998E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F12">
-        <f t="shared" ca="1" si="2"/>
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.33</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.34</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.16500000000000001</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.17</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4999999999999997E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="2"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.31</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.155</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="2"/>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.39</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.32</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.19500000000000001</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.16</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
@@ -783,33 +774,31 @@
         <v>5.5E-2</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="2"/>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.33</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.26</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.16500000000000001</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.13</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="2"/>
-        <v>101</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -817,24 +806,23 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.39</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.31</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.19500000000000001</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.155</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="E17">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
       <c r="F17">
-        <f t="shared" ca="1" si="2"/>
-        <v>103</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -842,24 +830,23 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.36</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.3</v>
       </c>
       <c r="C18">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.05</v>
+        <v>0.13</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5000000000000001E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F18">
-        <f t="shared" ca="1" si="2"/>
-        <v>117</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -867,12 +854,12 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.32</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.24</v>
       </c>
       <c r="C19">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.16</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.12</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
@@ -883,8 +870,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="F19">
-        <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -892,24 +878,23 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.31</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.33</v>
       </c>
       <c r="C20">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.155</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.03</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F20">
-        <f t="shared" ca="1" si="2"/>
-        <v>120</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -917,24 +902,23 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.37</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.2</v>
       </c>
       <c r="C21">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.185</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.1</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F21">
-        <f t="shared" ca="1" si="2"/>
-        <v>114</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -942,24 +926,23 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.25</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.22</v>
       </c>
       <c r="C22">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.125</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.11</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.13</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5000000000000003E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F22">
-        <f t="shared" ca="1" si="2"/>
-        <v>101</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -967,24 +950,23 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.31</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.3</v>
       </c>
       <c r="C23">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.155</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.05</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F23">
-        <f t="shared" ca="1" si="2"/>
-        <v>106</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -992,24 +974,23 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.38</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.37</v>
       </c>
       <c r="C24">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.19</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.185</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.12</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F24">
-        <f t="shared" ca="1" si="2"/>
-        <v>119</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1017,24 +998,28 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.25</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.35</v>
       </c>
       <c r="C25">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.125</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.17499999999999999</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.05</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F25">
-        <f t="shared" ca="1" si="2"/>
-        <v>90</v>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
carbon finally works fuck me
</commit_message>
<xml_diff>
--- a/markets.xlsx
+++ b/markets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheikh M Ahmed\modelling_MCDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CC71D5-2251-45C3-B8BE-06929D1CB89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFC6388-03F8-4701-A132-76E47D5EDB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{5524CA32-E132-410D-B865-513BEFDAB590}"/>
   </bookViews>
@@ -405,19 +405,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D915BB96-A88E-4797-BAC2-270B960E39C0}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="8.88671875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -437,117 +438,117 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(20,40)/100</f>
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
       <c r="C2">
         <f ca="1">B2*0.5</f>
-        <v>0.19500000000000001</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(5,15)/100</f>
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E2">
         <f ca="1">D2*0.5</f>
-        <v>0.06</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F2">
-        <v>0.1</v>
-      </c>
-      <c r="G2">
-        <f ca="1">RANDBETWEEN(90,120)</f>
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <f ca="1">RANDBETWEEN(6,20)/100</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <f ca="1">RANDBETWEEN(20,40)/100</f>
-        <v>0.34</v>
+        <v>0.4</v>
       </c>
       <c r="C3">
         <f ca="1">B3*0.5</f>
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D25" ca="1" si="0">RANDBETWEEN(5,15)/100</f>
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E25" ca="1" si="1">D3*0.5</f>
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="F3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ref="F3:F25" ca="1" si="2">RANDBETWEEN(6,20)/100</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B25" ca="1" si="2">RANDBETWEEN(20,40)/100</f>
-        <v>0.3</v>
+        <f t="shared" ref="B4:B25" ca="1" si="3">RANDBETWEEN(20,40)/100</f>
+        <v>0.34</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C25" ca="1" si="3">B4*0.5</f>
-        <v>0.15</v>
+        <f t="shared" ref="C4:C25" ca="1" si="4">B4*0.5</f>
+        <v>0.17</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.05</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.4</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.125</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="2"/>
         <v>0.06</v>
       </c>
-      <c r="F5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.28000000000000003</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.24</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.14000000000000001</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.12</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
@@ -558,140 +559,146 @@
         <v>0.04</v>
       </c>
       <c r="F6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.27</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0.13500000000000001</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
+        <v>0.06</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.03</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="2"/>
         <v>0.08</v>
       </c>
-      <c r="E7">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.04</v>
-      </c>
-      <c r="F7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.36</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.2</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.18</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.1</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F8">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.4</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.38</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.19</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15</v>
+        <v>0.06</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4999999999999997E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F9">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.35</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.39</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.17499999999999999</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.19500000000000001</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5000000000000002E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F10">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.28000000000000003</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.27</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.14000000000000001</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.06</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F11">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.32</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.39</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.16</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.19500000000000001</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
@@ -702,68 +709,71 @@
         <v>5.5E-2</v>
       </c>
       <c r="F12">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.39</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.26</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.19500000000000001</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.13</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4999999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F13">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.36</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.4</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.18</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.2</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.06</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F14">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.38</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.32</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.19</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.16</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
@@ -774,31 +784,33 @@
         <v>5.5E-2</v>
       </c>
       <c r="F15">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.36</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.26</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.18</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.13</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F16">
-        <v>0.2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.15</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -806,23 +818,24 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.35</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.24</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.17499999999999999</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.12</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.06</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F17">
-        <v>0.2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.13</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -830,23 +843,24 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.25</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C18">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11</v>
+        <v>0.05</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F18">
-        <v>0.2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -854,23 +868,24 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.38</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.31</v>
       </c>
       <c r="C19">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.19</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.155</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.03</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F19">
-        <v>0.2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -878,23 +893,24 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.31</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.37</v>
       </c>
       <c r="C20">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.155</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.185</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.05</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F20">
-        <v>0.2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.09</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -902,23 +918,24 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.35</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.2</v>
       </c>
       <c r="C21">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.17499999999999999</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.1</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="F21">
-        <v>0.1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -926,23 +943,24 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.21</v>
       </c>
       <c r="C22">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.15</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.105</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F22">
-        <v>0.1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.19</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -950,23 +968,24 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.39</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.27</v>
       </c>
       <c r="C23">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.19500000000000001</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F23">
-        <v>0.1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.17</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -974,12 +993,12 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.25</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.26</v>
       </c>
       <c r="C24">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.13</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
@@ -990,7 +1009,8 @@
         <v>0.06</v>
       </c>
       <c r="F24">
-        <v>0.1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.11</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -998,28 +1018,24 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.32</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.37</v>
       </c>
       <c r="C25">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.16</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.185</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F25">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F26">
-        <v>0.1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>